<commit_message>
Updated name in marks file
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicen\git\algorithmicsGarciaDiazVicenteUO42478\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO257850\OneDrive - Universidad de Oviedo\clase\Algoritmia\workspace\algorithmicsCampaMartinezUO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD47017-13A3-40B4-A991-1C202C3B8F53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052E0F11-28C5-431A-BB50-A1E812AE6242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24285" yWindow="3105" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Please, don't change this file after you indicate your name</t>
   </si>
   <si>
-    <t>García Díaz, Vicente</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Total maximum possible </t>
     </r>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>Each session will be graded with a score between 0 and 10</t>
+  </si>
+  <si>
+    <t>Campa Martínez, Armando</t>
   </si>
 </sst>
 </file>
@@ -874,52 +874,52 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>2</v>
@@ -928,9 +928,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -942,7 +942,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -952,7 +952,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -962,7 +962,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -972,7 +972,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -982,7 +982,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -992,7 +992,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1002,7 +1002,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1012,7 +1012,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1022,150 +1022,150 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I5:I12"/>

</xml_diff>

<commit_message>
Session 0 1.1 1.2
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO257850\OneDrive - Universidad de Oviedo\clase\Algoritmia\workspace\algorithmicsCampaMartinezUO257850\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052E0F11-28C5-431A-BB50-A1E812AE6242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF85BD7A-DEE8-484E-B7A9-211F3A4EFC72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24285" yWindow="3105" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Student</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Campa Martínez, Armando</t>
+  </si>
+  <si>
+    <t>Mark (scale 1-10)</t>
+  </si>
+  <si>
+    <t>Please, submit PDF files, not Word files. There were 2 activities in session 0 and some of the other exercises were quite incomplete. Tables and graphs should be included in the PDF doucment as requested</t>
   </si>
 </sst>
 </file>
@@ -257,7 +263,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -302,11 +308,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,19 +338,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="8"/>
@@ -341,12 +363,27 @@
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -532,19 +569,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla14515" displayName="Tabla14515" ref="A3:J4" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A3:J4" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Student" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Session 0, 1.1, 1.2" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Session 2 (Sorting)" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Session 3 (D&amp;C)" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Session 4 (Greedy)" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Session 5 (Dynamic Prog.)" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Session 6 (Backtracking)" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Session 7 (Branch&amp;Bound)" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Test mark" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Final mark" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla14515" displayName="Tabla14515" ref="A3:K4" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K4" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Student" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Session 0, 1.1, 1.2" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Session 2 (Sorting)" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Session 3 (D&amp;C)" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Session 4 (Greedy)" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Session 5 (Dynamic Prog.)" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Session 6 (Backtracking)" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Session 7 (Branch&amp;Bound)" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Test mark" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mark (scale 1-10)" dataDxfId="1">
+      <calculatedColumnFormula>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="1" xr3:uid="{52100805-9400-48F6-BD1A-0901CEDA56E9}" name="Final mark" dataDxfId="0">
+      <calculatedColumnFormula>IF(AND(J4&gt;=9,J4&lt;=10),7, IF(AND(J4&gt;=8,J4&lt;9),6.5, IF(AND(J4&gt;=7,J4&lt;8),6, IF(AND(J4&gt;=6,J4&lt;7),5.5, IF(AND(J4&gt;=5,J4&lt;6),5,4)))))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,32 +913,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J136"/>
+  <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.88671875" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,14 +967,19 @@
         <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>6</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -940,10 +987,19 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+      <c r="J4" s="11">
+        <f>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K4" s="12">
+        <f>IF(AND(J4&gt;=9,J4&lt;=10),7, IF(AND(J4&gt;=8,J4&lt;9),6.5, IF(AND(J4&gt;=7,J4&lt;8),6, IF(AND(J4&gt;=6,J4&lt;7),5.5, IF(AND(J4&gt;=5,J4&lt;6),5,4)))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -952,7 +1008,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -962,7 +1018,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -972,7 +1028,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -982,7 +1038,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -992,7 +1048,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1002,7 +1058,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1012,7 +1068,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1022,150 +1078,150 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I5:I12"/>

</xml_diff>

<commit_message>
Algorithms and automation coded
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/uo257850_uniovi_es/Documents/clase/Algoritmia/workspace/algorithmicsCampaMartinezUO257850/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF85BD7A-DEE8-484E-B7A9-211F3A4EFC72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EF85BD7A-DEE8-484E-B7A9-211F3A4EFC72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6DB0F7F3-0110-4BB6-B55B-1E7642CCAA41}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
@@ -338,6 +338,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -347,8 +349,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,29 +916,29 @@
   <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C12"/>
+      <selection activeCell="B5" sqref="B5:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -987,241 +987,241 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <f>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="9">
         <f>IF(AND(J4&gt;=9,J4&lt;=10),7, IF(AND(J4&gt;=8,J4&lt;9),6.5, IF(AND(J4&gt;=7,J4&lt;8),6, IF(AND(J4&gt;=6,J4&lt;7),5.5, IF(AND(J4&gt;=5,J4&lt;6),5,4)))))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I5:I12"/>

</xml_diff>

<commit_message>
Session 3: Divide and Conquer
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBF0201-C670-48D6-A3E1-A7E0B17E1A29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437288AE-09A7-4914-8555-B971B3A846E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="3615" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Student</t>
   </si>
@@ -215,6 +215,10 @@
   </si>
   <si>
     <t>Selection is not working for some cases and quicksort for the central element as the pivot is not implemented. You had to include the theoretical times (at least a couple of examples for each table) to compare the expirical results with the theoretical ones.</t>
+  </si>
+  <si>
+    <t>The D&amp;C version is not working as expected. It works but the complexity is not O(nlogn). Please, check the video of the last seminar (the implementation should be very similar to Mergesort).
+Nevative number of inversions are because you should use long instead of int (there are very large results).</t>
   </si>
 </sst>
 </file>
@@ -919,7 +923,7 @@
   <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -986,7 +990,9 @@
       <c r="C4" s="4">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>7</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -994,7 +1000,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="8">
         <f>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</f>
-        <v>1.3000000000000003</v>
+        <v>2.2310000000000003</v>
       </c>
       <c r="K4" s="9">
         <f>IF(AND(J4&gt;=9,J4&lt;=10),7, IF(AND(J4&gt;=8,J4&lt;9),6.5, IF(AND(J4&gt;=7,J4&lt;8),6, IF(AND(J4&gt;=6,J4&lt;7),5.5, IF(AND(J4&gt;=5,J4&lt;6),5,4)))))</f>
@@ -1008,7 +1014,9 @@
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1075,7 +1083,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:11" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>

</xml_diff>

<commit_message>
Session 4: Greedy algorithms
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437288AE-09A7-4914-8555-B971B3A846E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE30E157-CF8E-4726-BA39-EAD2CE222AE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Student</t>
   </si>
@@ -219,6 +219,9 @@
   <si>
     <t>The D&amp;C version is not working as expected. It works but the complexity is not O(nlogn). Please, check the video of the last seminar (the implementation should be very similar to Mergesort).
 Nevative number of inversions are because you should use long instead of int (there are very large results).</t>
+  </si>
+  <si>
+    <t>Algorithms didn't give correct results and the expected complexity for greedy 2 and greedy 3 is O(nlogn) if you sort the elements beforehand or if you use a priority queue</t>
   </si>
 </sst>
 </file>
@@ -923,7 +926,7 @@
   <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D12"/>
+      <selection activeCell="E5" sqref="E5:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -993,14 +996,16 @@
       <c r="D4" s="4">
         <v>7</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="8">
         <f>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</f>
-        <v>2.2310000000000003</v>
+        <v>2.7630000000000003</v>
       </c>
       <c r="K4" s="9">
         <f>IF(AND(J4&gt;=9,J4&lt;=10),7, IF(AND(J4&gt;=8,J4&lt;9),6.5, IF(AND(J4&gt;=7,J4&lt;8),6, IF(AND(J4&gt;=6,J4&lt;7),5.5, IF(AND(J4&gt;=5,J4&lt;6),5,4)))))</f>
@@ -1017,7 +1022,9 @@
       <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>

</xml_diff>

<commit_message>
Session 5: Dynamic Programming
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE30E157-CF8E-4726-BA39-EAD2CE222AE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4878AD1E-743C-499B-9680-27632817AFC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Student</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Algorithms didn't give correct results and the expected complexity for greedy 2 and greedy 3 is O(nlogn) if you sort the elements beforehand or if you use a priority queue</t>
+  </si>
+  <si>
+    <t>No new files included</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
   <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E12"/>
+      <selection activeCell="G5" sqref="G5:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -999,7 +1002,9 @@
       <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1025,7 +1030,9 @@
       <c r="E5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>

</xml_diff>

<commit_message>
Session 7: Branch and Bound
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\alg-1-CampaMartínezArmando-UO257850\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620614BA-0297-47A5-8D4C-05AA3239B741}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8399D7-2DC0-4E7A-8C17-BBA336A37C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Student</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>No new files included</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -928,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -944,6 +947,7 @@
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1008,8 +1012,12 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="J4" s="8">
         <f>(B4*0.1+C4*0.1+D4*0.133+E4*0.133+F4*0.134+G4*0.2+H4*0.2)</f>
         <v>2.7630000000000003</v>
@@ -1038,7 +1046,9 @@
       <c r="G5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>